<commit_message>
Added toggling between celery/redis/rabbitmq and not
</commit_message>
<xml_diff>
--- a/AlchemyApp/static/Assessment_Workbook_with_Analysis.xlsx
+++ b/AlchemyApp/static/Assessment_Workbook_with_Analysis.xlsx
@@ -18920,7 +18920,7 @@
       </c>
       <c r="H21" s="89" t="inlineStr">
         <is>
-          <t>The document clearly states that Purdue Pharma will document and monitor individual information system security training activities, which includes basic security awareness training and specific information system security training. However, the document does not mention anything about privacy training activities.</t>
+          <t>The document outlines that Purdue Pharma will document and monitor individual information system security training activities, including basic security awareness training and specific information system security training. However, there is no mention of privacy training activities, including privacy awareness training and specific role-based privacy training.</t>
         </is>
       </c>
       <c r="I21" s="46" t="inlineStr">
@@ -18930,12 +18930,12 @@
       </c>
       <c r="J21" s="89" t="inlineStr">
         <is>
-          <t>The document should include a section that specifically addresses privacy training activities. This section should state that Purdue Pharma will document and monitor individual information privacy training activities, which includes basic privacy awareness training and specific role-based privacy training.</t>
+          <t>The policy should be updated to include provisions for documenting and monitoring privacy training activities, including privacy awareness training and specific role-based privacy training.</t>
         </is>
       </c>
       <c r="K21" s="89" t="inlineStr">
         <is>
-          <t>"PRIVACY TRAINING RECORDS Purdue Pharma shall: a.Designate personnel to document and monitor individual information privacy training activities including basic privacy awareness training and specific role-based privacy training. b.Retain individual privacy training records for six years."</t>
+          <t>"SECURITY AND PRIVACY TRAINING RECORDS Purdue Pharma shall: a.Designate personnel to document and monitor individual information system security and privacy training activities including basic security and privacy awareness training and specific information system security and role-based privacy training. b.Retain individual training records for six years."</t>
         </is>
       </c>
     </row>
@@ -18977,7 +18977,7 @@
       </c>
       <c r="H22" s="89" t="inlineStr">
         <is>
-          <t>The document meets the requirements of the given test procedure. It states that individual training records are retained, and the retention period is six years, which is significantly longer than the one year specified in the test procedure.</t>
+          <t>The document meets the requirements of the given test procedure. It states that Purdue Pharma will retain individual training records for six years, which is significantly longer than the one year required by the test procedure.</t>
         </is>
       </c>
       <c r="I22" s="46" t="inlineStr">

</xml_diff>

<commit_message>
Updating to latest version before DK
</commit_message>
<xml_diff>
--- a/AlchemyApp/static/Assessment_Workbook_with_Analysis.xlsx
+++ b/AlchemyApp/static/Assessment_Workbook_with_Analysis.xlsx
@@ -18276,12 +18276,28 @@
           <t>Determine if an awareness and training policy is developed, documented and disseminated to organization-defined personnel or roles.</t>
         </is>
       </c>
-      <c r="F2" s="77" t="n"/>
-      <c r="G2" s="77" t="n"/>
-      <c r="H2" s="77" t="n"/>
-      <c r="I2" s="46" t="n"/>
-      <c r="J2" s="77" t="n"/>
-      <c r="K2" s="77" t="n"/>
+      <c r="F2" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G2" s="89" t="inlineStr">
+        <is>
+          <t>The relevant sections of text that offer evidence to support that the test requirement is implemented are: "SECURITY AWARENESS TRAINING Purdue Pharma shall: a.Schedule security awareness training as part of initial training for new users. b.Schedule security awareness training when required by information system changes and then every two years thereafter. c.IT shall determine the appropriate content of security awareness training and security awareness techniques based on the specific organizational requirements and the information systems to which personnel have authorized access." and "COMPLIANCE Employees who violate this policy may be subject to appropriate disciplinary action up to and including discharge as well as both civil and criminal penalties."</t>
+        </is>
+      </c>
+      <c r="H2" s="89" t="inlineStr">
+        <is>
+          <t>The document meets the requirements of the given test procedure well. It clearly states that Purdue Pharma has developed a security awareness training policy, which is scheduled for new users, when required by system changes, and every two years thereafter. The IT department determines the content of the training based on organizational requirements and the systems to which personnel have access. The policy is also disseminated to personnel, as evidenced by the compliance section which outlines penalties for violation of the policy.</t>
+        </is>
+      </c>
+      <c r="I2" s="46" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="J2" s="89" t="inlineStr"/>
+      <c r="K2" s="89" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="49" t="inlineStr">
@@ -18309,12 +18325,28 @@
           <t>Determine if awareness and training procedures to facilitate the implementation of the awareness and training policy and associated awareness and training controls are developed, documented and disseminated to organization-defined personnel or roles.</t>
         </is>
       </c>
-      <c r="F3" s="77" t="n"/>
-      <c r="G3" s="77" t="n"/>
-      <c r="H3" s="77" t="n"/>
-      <c r="I3" s="46" t="n"/>
-      <c r="J3" s="77" t="n"/>
-      <c r="K3" s="77" t="n"/>
+      <c r="F3" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G3" s="89" t="inlineStr">
+        <is>
+          <t>The relevant sections of text that offer evidence to support that the test requirement is implemented are: "SECURITY AWARENESS TRAINING Purdue Pharma shall: a.Schedule security awareness training as part of initial training for new users. b.Schedule security awareness training when required by information system changes and then every two years thereafter. c.IT shall determine the appropriate content of security awareness training and security awareness techniques based on the specific organizational requirements and the information systems to which personnel have authorized access." and "SECURITY TRAINING RECORDS Purdue Pharma shall: a.Designate personnel to document and monitor individual information system security training activities including basic security awareness training and specific information system security training. b.Retain individual training records for six years."</t>
+        </is>
+      </c>
+      <c r="H3" s="89" t="inlineStr">
+        <is>
+          <t>The document meets the requirements of the given test procedure well. It clearly states that Purdue Pharma schedules security awareness training for new users and every two years thereafter. It also mentions that the IT department determines the content of the training based on organizational requirements and the systems to which personnel have access. Furthermore, the document states that Purdue Pharma designates personnel to document and monitor security training activities and retains these records for six years.</t>
+        </is>
+      </c>
+      <c r="I3" s="46" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="J3" s="89" t="inlineStr"/>
+      <c r="K3" s="89" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="49" t="inlineStr">
@@ -18342,12 +18374,28 @@
           <t>Determine if the organizational-level, mission/business process-level, or system-level awareness and training policy addresses purpose, scope, roles, responsibilities, management commitment, coordination among organizational entities, and compliance.</t>
         </is>
       </c>
-      <c r="F4" s="77" t="n"/>
-      <c r="G4" s="77" t="n"/>
-      <c r="H4" s="77" t="n"/>
-      <c r="I4" s="46" t="n"/>
-      <c r="J4" s="77" t="n"/>
-      <c r="K4" s="77" t="n"/>
+      <c r="F4" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G4" s="89" t="inlineStr">
+        <is>
+          <t>The document addresses purpose ("To ensure that the appropriate level of information security awareness training is provided to all Information Technology (IT) users."), scope (applicable to all departments and users of IT resources and assets), roles (IT Department, Chief Information Office), responsibilities (security awareness training, recognizing suspicious communications, documenting and monitoring training activities), management commitment (policy enforced by disciplinary action, civil and criminal penalties), coordination among organizational entities (requests for exceptions reviewed by CISO and CIO), and compliance (employees subject to disciplinary action, non-employees subject to termination of contractual agreements, denial of access to IT resources).</t>
+        </is>
+      </c>
+      <c r="H4" s="89" t="inlineStr">
+        <is>
+          <t>The document meets the requirements of the test procedure well. It clearly outlines the purpose, scope, roles, responsibilities, management commitment, coordination among organizational entities, and compliance.</t>
+        </is>
+      </c>
+      <c r="I4" s="46" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="J4" s="89" t="inlineStr"/>
+      <c r="K4" s="89" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="49" t="inlineStr">
@@ -18375,12 +18423,28 @@
           <t>Determine if the awareness and training policy is consistent with applicable laws, Executive Orders, directives, regulations, policies, standards, and guidelines.</t>
         </is>
       </c>
-      <c r="F5" s="77" t="n"/>
-      <c r="G5" s="77" t="n"/>
-      <c r="H5" s="77" t="n"/>
-      <c r="I5" s="46" t="n"/>
-      <c r="J5" s="77" t="n"/>
-      <c r="K5" s="77" t="n"/>
+      <c r="F5" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G5" s="89" t="inlineStr">
+        <is>
+          <t>The document references "National Institute of Standards and Technology (NIST) Special Publications: NIST SP 800-53 – Awareness and Training (AT), NIST SP 800-12, NIST SP 800-16, NIST SP 800-50, NIST SP 800-100; Electronic Code of Federal Regulations (CFR): 5 CFR 930.301". It also mentions that "This policy is applicable to all departments and users of IT resources and assets" and outlines the security awareness training and insider threat training that Purdue Pharma shall provide. It also states that "Employees who violate this policy may be subject to appropriate disciplinary action up to and including discharge as well as both civil and criminal penalties."</t>
+        </is>
+      </c>
+      <c r="H5" s="89" t="inlineStr">
+        <is>
+          <t>The document appears to be consistent with applicable laws, Executive Orders, directives, regulations, policies, standards, and guidelines. It references NIST publications and the Electronic Code of Federal Regulations, which are standard guidelines for information security. It also outlines the training that will be provided, the consequences for violating the policy, and the process for requesting exceptions to the policy.</t>
+        </is>
+      </c>
+      <c r="I5" s="46" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="J5" s="89" t="inlineStr"/>
+      <c r="K5" s="89" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="49" t="inlineStr">
@@ -18408,12 +18472,36 @@
           <t>Determine if the organization-defined official is designated to manage the development, documentation, and dissemination of the awareness and training policy and procedures.</t>
         </is>
       </c>
-      <c r="F6" s="77" t="n"/>
-      <c r="G6" s="77" t="n"/>
-      <c r="H6" s="77" t="n"/>
-      <c r="I6" s="46" t="n"/>
-      <c r="J6" s="77" t="n"/>
-      <c r="K6" s="77" t="n"/>
+      <c r="F6" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G6" s="89" t="inlineStr">
+        <is>
+          <t>"SECURITY TRAINING RECORDS Purdue Pharma shall: a.Designate personnel to document and monitor individual information system security training activities including basic security awareness training and specific information system security training."</t>
+        </is>
+      </c>
+      <c r="H6" s="89" t="inlineStr">
+        <is>
+          <t>The document does indicate that Purdue Pharma designates personnel to manage the documentation and monitoring of security training activities. However, it does not explicitly state that this designated official is also responsible for the development and dissemination of the awareness and training policy and procedures.</t>
+        </is>
+      </c>
+      <c r="I6" s="46" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J6" s="89" t="inlineStr">
+        <is>
+          <t>The policy should be updated to explicitly state that the designated official is responsible for the development, documentation, and dissemination of the awareness and training policy and procedures.</t>
+        </is>
+      </c>
+      <c r="K6" s="89" t="inlineStr">
+        <is>
+          <t>"SECURITY TRAINING RECORDS Purdue Pharma shall: a. Designate an organization-defined official to manage the development, documentation, dissemination, and monitoring of individual information system security training activities including basic security awareness training and specific information system security training."</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="49" t="inlineStr">
@@ -18441,12 +18529,36 @@
           <t>Determine if the current awareness and training policy is reviewed and updated at least every three (3) years as well as after significant changes to in-scope systems.</t>
         </is>
       </c>
-      <c r="F7" s="77" t="n"/>
-      <c r="G7" s="77" t="n"/>
-      <c r="H7" s="77" t="n"/>
-      <c r="I7" s="46" t="n"/>
-      <c r="J7" s="77" t="n"/>
-      <c r="K7" s="77" t="n"/>
+      <c r="F7" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G7" s="89" t="inlineStr">
+        <is>
+          <t>"Date Issued:12/01/2019Date Reviewed:12/01/2020"</t>
+        </is>
+      </c>
+      <c r="H7" s="89" t="inlineStr">
+        <is>
+          <t>The document indicates that the policy was reviewed one year after it was issued. However, there is no explicit mention of a policy to review and update the awareness and training policy at least every three years or after significant changes to in-scope systems.</t>
+        </is>
+      </c>
+      <c r="I7" s="46" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J7" s="89" t="inlineStr">
+        <is>
+          <t>The policy should be updated to explicitly state that it will be reviewed and updated at least every three years and after significant changes to in-scope systems. This will ensure that the policy remains relevant and effective in managing the information security risks associated with changes in technology, threats, business operations, or the regulatory environment.</t>
+        </is>
+      </c>
+      <c r="K7" s="89" t="inlineStr">
+        <is>
+          <t>"This policy will be reviewed and updated at least every three years and after significant changes to in-scope systems to ensure that it remains relevant and effective in managing the information security risks associated with changes in technology, threats, business operations, or the regulatory environment. Date Issued: 12/01/2019. Last Reviewed: 12/01/2020. Next Scheduled Review: 12/01/2022 or after significant changes to in-scope systems, whichever comes first."</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="49" t="inlineStr">
@@ -18474,12 +18586,36 @@
           <t>Determine if the current awareness and training procedures are reviewed and updated at least annually as well as after significant changes to in-scope systems.</t>
         </is>
       </c>
-      <c r="F8" s="77" t="n"/>
-      <c r="G8" s="77" t="n"/>
-      <c r="H8" s="77" t="n"/>
-      <c r="I8" s="46" t="n"/>
-      <c r="J8" s="77" t="n"/>
-      <c r="K8" s="77" t="n"/>
+      <c r="F8" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G8" s="89" t="inlineStr">
+        <is>
+          <t>"Schedule security awareness training when required by information system changes and then every two years thereafter." "Date Issued:12/01/2019Date Reviewed:12/01/2020"</t>
+        </is>
+      </c>
+      <c r="H8" s="89" t="inlineStr">
+        <is>
+          <t>The document indicates that security awareness training is scheduled when required by information system changes and then every two years thereafter. However, it does not explicitly state that the awareness and training procedures are reviewed and updated at least annually. The document was reviewed a year after it was issued, but it is unclear if this review included an update of the training procedures.</t>
+        </is>
+      </c>
+      <c r="I8" s="46" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J8" s="89" t="inlineStr">
+        <is>
+          <t>The policy should be updated to explicitly state that the awareness and training procedures are reviewed and updated at least annually and after significant changes to in-scope systems. This will ensure that the training procedures remain relevant and effective.</t>
+        </is>
+      </c>
+      <c r="K8" s="89" t="inlineStr">
+        <is>
+          <t>"Purdue Pharma shall: a. Schedule security awareness training as part of initial training for new users. b. Schedule security awareness training when required by information system changes and then every two years thereafter. c. Review and update the awareness and training procedures at least annually and after significant changes to in-scope systems."</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="49" t="inlineStr">
@@ -18507,12 +18643,36 @@
           <t>Determine if security literacy training is provided to system users (including managers, senior executives, and contractors) as part of initial training for new users and at least annually thereafter.</t>
         </is>
       </c>
-      <c r="F9" s="77" t="n"/>
-      <c r="G9" s="77" t="n"/>
-      <c r="H9" s="77" t="n"/>
-      <c r="I9" s="46" t="n"/>
-      <c r="J9" s="77" t="n"/>
-      <c r="K9" s="77" t="n"/>
+      <c r="F9" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G9" s="89" t="inlineStr">
+        <is>
+          <t>"SECURITY AWARENESS TRAINING Purdue Pharma shall: a.Schedule security awareness training as part of initial training for new users. b.Schedule security awareness training when required by information system changes and then every two years thereafter."</t>
+        </is>
+      </c>
+      <c r="H9" s="89" t="inlineStr">
+        <is>
+          <t>The document states that security awareness training is provided as part of initial training for new users, which meets part of the test requirement. However, the document specifies that subsequent training is scheduled every two years, not annually as the test procedure requires.</t>
+        </is>
+      </c>
+      <c r="I9" s="46" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J9" s="89" t="inlineStr">
+        <is>
+          <t>Purdue Pharma should revise its policy to include annual security awareness training for all system users, including managers, senior executives, and contractors, to meet the test procedure requirement.</t>
+        </is>
+      </c>
+      <c r="K9" s="89" t="inlineStr">
+        <is>
+          <t>"SECURITY AWARENESS TRAINING Purdue Pharma shall: a.Schedule security awareness training as part of initial training for new users. b.Schedule annual security awareness training for all system users, including managers, senior executives, and contractors, and additional training when required by information system changes."</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="49" t="inlineStr">
@@ -18540,12 +18700,36 @@
           <t>Determine if privacy literacy training is provided to system users (including managers, senior executives, and contractors) as part of initial training for new users and at least annually thereafter.</t>
         </is>
       </c>
-      <c r="F10" s="77" t="n"/>
-      <c r="G10" s="77" t="n"/>
-      <c r="H10" s="77" t="n"/>
-      <c r="I10" s="46" t="n"/>
-      <c r="J10" s="77" t="n"/>
-      <c r="K10" s="77" t="n"/>
+      <c r="F10" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G10" s="89" t="inlineStr">
+        <is>
+          <t>"SECURITY AWARENESS TRAINING Purdue Pharma shall: a.Schedule security awareness training as part of initial training for new users. b.Schedule security awareness training when required by information system changes and then every two years thereafter."</t>
+        </is>
+      </c>
+      <c r="H10" s="89" t="inlineStr">
+        <is>
+          <t>The document mentions that Purdue Pharma schedules security awareness training for new users and every two years thereafter. However, it does not specifically mention privacy literacy training or that such training is provided at least annually.</t>
+        </is>
+      </c>
+      <c r="I10" s="46" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J10" s="89" t="inlineStr">
+        <is>
+          <t>Purdue Pharma should include privacy literacy training as part of the initial training for new users and ensure that this training is provided at least annually. This training should be extended to all system users, including managers, senior executives, and contractors.</t>
+        </is>
+      </c>
+      <c r="K10" s="89" t="inlineStr">
+        <is>
+          <t>"SECURITY AWARENESS TRAINING Purdue Pharma shall: a.Schedule security awareness and privacy literacy training as part of initial training for new users. b.Schedule security awareness and privacy literacy training when required by information system changes and at least annually thereafter. This training should be extended to all system users, including managers, senior executives, and contractors."</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="49" t="inlineStr">
@@ -18574,12 +18758,36 @@
 Additionally, determine if  privacy literacy training is provided to system users (including managers, senior executives, and contractors) when required by system changes or following organization-defined events.</t>
         </is>
       </c>
-      <c r="F11" s="77" t="n"/>
-      <c r="G11" s="77" t="n"/>
-      <c r="H11" s="77" t="n"/>
-      <c r="I11" s="46" t="n"/>
-      <c r="J11" s="77" t="n"/>
-      <c r="K11" s="77" t="n"/>
+      <c r="F11" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G11" s="89" t="inlineStr">
+        <is>
+          <t>"SECURITY AWARENESS TRAINING Purdue Pharma shall: b.Schedule security awareness training when required by information system changes and then every two years thereafter. c.IT shall determine the appropriate content of security awareness training and security awareness techniques based on the specific organizational requirements and the information systems to which personnel have authorized access."</t>
+        </is>
+      </c>
+      <c r="H11" s="89" t="inlineStr">
+        <is>
+          <t>The document indicates that Purdue Pharma schedules security awareness training when required by information system changes. However, it does not specifically mention privacy literacy training or that this training is provided to all system users including managers, senior executives, and contractors.</t>
+        </is>
+      </c>
+      <c r="I11" s="46" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J11" s="89" t="inlineStr">
+        <is>
+          <t>The policy should be updated to explicitly state that privacy literacy training is provided to all system users, including managers, senior executives, and contractors, when required by system changes or following organization-defined events.</t>
+        </is>
+      </c>
+      <c r="K11" s="89" t="inlineStr">
+        <is>
+          <t>"SECURITY AND PRIVACY AWARENESS TRAINING Purdue Pharma shall: b.Schedule security and privacy awareness training when required by information system changes and then every two years thereafter. c.IT shall determine the appropriate content of security and privacy awareness training and security awareness techniques based on the specific organizational requirements and the information systems to which personnel have authorized access. This training shall be provided to all system users, including managers, senior executives, and contractors."</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="49" t="inlineStr">
@@ -18608,12 +18816,36 @@
 Additionally, determine if organization-defined awareness techniques are employed to increase the privacy awareness of system users.</t>
         </is>
       </c>
-      <c r="F12" s="77" t="n"/>
-      <c r="G12" s="77" t="n"/>
-      <c r="H12" s="77" t="n"/>
-      <c r="I12" s="46" t="n"/>
-      <c r="J12" s="77" t="n"/>
-      <c r="K12" s="77" t="n"/>
+      <c r="F12" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G12" s="89" t="inlineStr">
+        <is>
+          <t>The relevant sections of text that offer evidence to support that the test requirement is implemented are: "IT shall determine the appropriate content of security awareness training and security awareness techniques based on the specific organizational requirements and the information systems to which personnel have authorized access. The content shall: i.Include a basic understanding of the need for information security and user actions to maintain security and to respond to suspected security incidents. ii.Address awareness of the need for operations security. Security awareness techniques can include, for example, displaying posters, offering supplies inscribed with security reminders, generating email advisories/notices from senior organizational officials, displaying logon screen messages, and conducting information security awareness events."</t>
+        </is>
+      </c>
+      <c r="H12" s="89" t="inlineStr">
+        <is>
+          <t>The document meets the requirements of the given test procedure to a certain extent. It mentions that the organization uses various techniques to increase the security awareness of system users. However, it does not explicitly mention any techniques employed to increase the privacy awareness of system users.</t>
+        </is>
+      </c>
+      <c r="I12" s="46" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J12" s="89" t="inlineStr">
+        <is>
+          <t>The organization should include specific techniques that are employed to increase the privacy awareness of system users in the policy document. This could include privacy training sessions, privacy reminders, and privacy awareness events.</t>
+        </is>
+      </c>
+      <c r="K12" s="89" t="inlineStr">
+        <is>
+          <t>The updated text could look like: "The content shall: i.Include a basic understanding of the need for information security and user actions to maintain security and to respond to suspected security incidents. ii.Address awareness of the need for operations security and privacy. Security and privacy awareness techniques can include, for example, displaying posters, offering supplies inscribed with security and privacy reminders, generating email advisories/notices from senior organizational officials, displaying logon screen messages, conducting information security and privacy awareness events."</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="49" t="inlineStr">
@@ -18641,12 +18873,36 @@
           <t>Determine if literacy training and awareness content is updated at least annually and after significant changes. This is different than if the training is being executed - is the content actually being updated?</t>
         </is>
       </c>
-      <c r="F13" s="77" t="n"/>
-      <c r="G13" s="77" t="n"/>
-      <c r="H13" s="77" t="n"/>
-      <c r="I13" s="46" t="n"/>
-      <c r="J13" s="77" t="n"/>
-      <c r="K13" s="77" t="n"/>
+      <c r="F13" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G13" s="89" t="inlineStr">
+        <is>
+          <t>"Schedule security awareness training when required by information system changes and then every two years thereafter." "IT shall determine the appropriate content of security awareness training and security awareness techniques based on the specific organizational requirements and the information systems to which personnel have authorized access."</t>
+        </is>
+      </c>
+      <c r="H13" s="89" t="inlineStr">
+        <is>
+          <t>The document mentions that security awareness training is scheduled when required by information system changes and then every two years thereafter. It also states that IT determines the appropriate content of security awareness training based on specific organizational requirements and the information systems to which personnel have access. However, it does not explicitly state that the content is updated at least annually or after significant changes.</t>
+        </is>
+      </c>
+      <c r="I13" s="46" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J13" s="89" t="inlineStr">
+        <is>
+          <t>The policy should be updated to explicitly state that the content of the security awareness training is updated at least annually and after significant changes to the information system.</t>
+        </is>
+      </c>
+      <c r="K13" s="89" t="inlineStr">
+        <is>
+          <t>"IT shall determine the appropriate content of security awareness training and security awareness techniques based on the specific organizational requirements and the information systems to which personnel have authorized access. The content shall be updated at least annually and after significant changes to the information system."</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="49" t="inlineStr">
@@ -18674,12 +18930,36 @@
           <t>Determine if lessons learned from internal or external security incidents or breaches are incorporated into literacy training and awareness techniques</t>
         </is>
       </c>
-      <c r="F14" s="77" t="n"/>
-      <c r="G14" s="77" t="n"/>
-      <c r="H14" s="77" t="n"/>
-      <c r="I14" s="46" t="n"/>
-      <c r="J14" s="77" t="n"/>
-      <c r="K14" s="77" t="n"/>
+      <c r="F14" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G14" s="89" t="inlineStr">
+        <is>
+          <t>The document does not provide any specific sections that indicate lessons learned from internal or external security incidents or breaches are incorporated into literacy training and awareness techniques.</t>
+        </is>
+      </c>
+      <c r="H14" s="89" t="inlineStr">
+        <is>
+          <t>The document does not meet the requirements of the given test procedure as it does not mention the incorporation of lessons learned from security incidents into the training and awareness programs.</t>
+        </is>
+      </c>
+      <c r="I14" s="46" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J14" s="89" t="inlineStr">
+        <is>
+          <t>The organization should incorporate a section in the policy that specifically addresses the use of lessons learned from security incidents in the training and awareness programs. This could include regular updates to the training content based on recent incidents and the inclusion of case studies in the training materials.</t>
+        </is>
+      </c>
+      <c r="K14" s="89" t="inlineStr">
+        <is>
+          <t>"IT Department shall: a. Provide training to its specified staff on how to recognize suspicious communications and anomalous behavior in organizational information systems. b. Incorporate lessons learned from internal and external security incidents into the training and awareness programs. This could include regular updates to the training content based on recent incidents and the inclusion of case studies in the training materials."</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="49" t="inlineStr">
@@ -18707,12 +18987,28 @@
           <t>Determine if literacy training on recognizing and reporting potential indicators of insider threat is provided</t>
         </is>
       </c>
-      <c r="F15" s="77" t="n"/>
-      <c r="G15" s="77" t="n"/>
-      <c r="H15" s="77" t="n"/>
-      <c r="I15" s="46" t="n"/>
-      <c r="J15" s="77" t="n"/>
-      <c r="K15" s="77" t="n"/>
+      <c r="F15" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G15" s="89" t="inlineStr">
+        <is>
+          <t>"IT Department shall: a.Provide training to its specified staff on how to recognize suspicious communications and anomalous behavior in organizational information systems."</t>
+        </is>
+      </c>
+      <c r="H15" s="89" t="inlineStr">
+        <is>
+          <t>The document does meet the requirements of the given test procedure. It explicitly states that the IT Department is responsible for providing training to staff on recognizing suspicious communications and anomalous behavior, which are potential indicators of an insider threat.</t>
+        </is>
+      </c>
+      <c r="I15" s="46" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="J15" s="89" t="inlineStr"/>
+      <c r="K15" s="89" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="49" t="inlineStr">
@@ -18740,12 +19036,36 @@
           <t>Determine if literacy training on recognizing and reporting potential and actual instances of social engineering and social mining is provided</t>
         </is>
       </c>
-      <c r="F16" s="77" t="n"/>
-      <c r="G16" s="77" t="n"/>
-      <c r="H16" s="77" t="n"/>
-      <c r="I16" s="46" t="n"/>
-      <c r="J16" s="77" t="n"/>
-      <c r="K16" s="77" t="n"/>
+      <c r="F16" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G16" s="89" t="inlineStr">
+        <is>
+          <t>"IT Department shall: a.Provide training to its specified staff on how to recognize suspicious communications and anomalous behavior in organizational information systems."</t>
+        </is>
+      </c>
+      <c r="H16" s="89" t="inlineStr">
+        <is>
+          <t>The document mentions that the IT Department provides training to staff on recognizing suspicious communications and anomalous behavior. However, it does not specifically mention literacy training on recognizing and reporting potential and actual instances of social engineering and social mining.</t>
+        </is>
+      </c>
+      <c r="I16" s="46" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J16" s="89" t="inlineStr">
+        <is>
+          <t>The policy should be updated to specifically include literacy training on recognizing and reporting potential and actual instances of social engineering and social mining. This could be incorporated into the existing training provided by the IT Department.</t>
+        </is>
+      </c>
+      <c r="K16" s="89" t="inlineStr">
+        <is>
+          <t>"IT Department shall: a.Provide training to its specified staff on how to recognize suspicious communications, anomalous behavior, and potential and actual instances of social engineering and social mining in organizational information systems. Staff should also be trained on how to report these instances."</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="49" t="inlineStr">
@@ -18774,12 +19094,36 @@
 Additionally, determine if role-based privacy training is provided to organization-defined roles and responsibilities before authorizing access to the system, information, or performing assigned duties and at least annually thereafter.</t>
         </is>
       </c>
-      <c r="F17" s="77" t="n"/>
-      <c r="G17" s="77" t="n"/>
-      <c r="H17" s="77" t="n"/>
-      <c r="I17" s="46" t="n"/>
-      <c r="J17" s="77" t="n"/>
-      <c r="K17" s="77" t="n"/>
+      <c r="F17" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G17" s="89" t="inlineStr">
+        <is>
+          <t>"ROLE-BASED SECURITY TRAINING IT Department shall: a.Provide role-based security training to personnel with assigned security roles and responsibilities: i.Before authorizing access to the information system or performing assigned duties. ii.When required by information system changes and annually thereafter."</t>
+        </is>
+      </c>
+      <c r="H17" s="89" t="inlineStr">
+        <is>
+          <t>The document clearly states that role-based security training is provided to personnel with assigned security roles and responsibilities before authorizing access to the information system or performing assigned duties, and when required by information system changes and annually thereafter. This meets the requirements of the given test procedure for security training. However, there is no mention of role-based privacy training in the document.</t>
+        </is>
+      </c>
+      <c r="I17" s="46" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J17" s="89" t="inlineStr">
+        <is>
+          <t>The organization should include role-based privacy training in its policy. This training should be provided to personnel with assigned roles and responsibilities before authorizing access to the system, information, or performing assigned duties and at least annually thereafter.</t>
+        </is>
+      </c>
+      <c r="K17" s="89" t="inlineStr">
+        <is>
+          <t>"ROLE-BASED SECURITY AND PRIVACY TRAINING IT Department shall: a.Provide role-based security and privacy training to personnel with assigned security roles and responsibilities: i.Before authorizing access to the information system or performing assigned duties. ii.When required by information system changes and annually thereafter."</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="49" t="inlineStr">
@@ -18808,12 +19152,36 @@
 Additionally, determine if role-based privacy training is provided to personnel with assigned security roles and responsibilities when required by system changes</t>
         </is>
       </c>
-      <c r="F18" s="77" t="n"/>
-      <c r="G18" s="77" t="n"/>
-      <c r="H18" s="77" t="n"/>
-      <c r="I18" s="46" t="n"/>
-      <c r="J18" s="77" t="n"/>
-      <c r="K18" s="77" t="n"/>
+      <c r="F18" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G18" s="89" t="inlineStr">
+        <is>
+          <t>"ROLE-BASED SECURITY TRAINING IT Department shall: a.Provide role-based security training to personnel with assigned security roles and responsibilities: i.Before authorizing access to the information system or performing assigned duties. ii.When required by information system changes and annually thereafter."</t>
+        </is>
+      </c>
+      <c r="H18" s="89" t="inlineStr">
+        <is>
+          <t>The document clearly states that role-based security training is provided to personnel with assigned security roles and responsibilities when required by system changes. However, there is no mention of role-based privacy training in the document.</t>
+        </is>
+      </c>
+      <c r="I18" s="46" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J18" s="89" t="inlineStr">
+        <is>
+          <t>The document should include a provision for role-based privacy training for personnel with assigned security roles and responsibilities when required by system changes. This training should be similar to the role-based security training already in place.</t>
+        </is>
+      </c>
+      <c r="K18" s="89" t="inlineStr">
+        <is>
+          <t>"ROLE-BASED SECURITY AND PRIVACY TRAINING IT Department shall: a.Provide role-based security and privacy training to personnel with assigned security roles and responsibilities: i.Before authorizing access to the information system or performing assigned duties. ii.When required by information system changes and annually thereafter."</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="49" t="inlineStr">
@@ -18841,12 +19209,36 @@
           <t>Determine if role-based training content is updated at least annually and after organization-defined events. This is different than if the training is being executed - is the content actually being updated?</t>
         </is>
       </c>
-      <c r="F19" s="77" t="n"/>
-      <c r="G19" s="77" t="n"/>
-      <c r="H19" s="77" t="n"/>
-      <c r="I19" s="46" t="n"/>
-      <c r="J19" s="77" t="n"/>
-      <c r="K19" s="77" t="n"/>
+      <c r="F19" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G19" s="89" t="inlineStr">
+        <is>
+          <t>The document mentions "Schedule security awareness training when required by information system changes and then every two years thereafter." and "IT shall determine the appropriate content of security awareness training and security awareness techniques based on the specific organizational requirements and the information systems to which personnel have authorized access."</t>
+        </is>
+      </c>
+      <c r="H19" s="89" t="inlineStr">
+        <is>
+          <t>The document does not explicitly state that the role-based training content is updated at least annually or after organization-defined events. It only mentions that training is scheduled every two years or when required by system changes.</t>
+        </is>
+      </c>
+      <c r="I19" s="46" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J19" s="89" t="inlineStr">
+        <is>
+          <t>The policy should be updated to explicitly state that role-based training content is updated at least annually and after organization-defined events. This will ensure that the training content remains relevant and up-to-date with the latest security threats and best practices.</t>
+        </is>
+      </c>
+      <c r="K19" s="89" t="inlineStr">
+        <is>
+          <t>The updated text could be: "IT shall determine the appropriate content of security awareness training and security awareness techniques based on the specific organizational requirements and the information systems to which personnel have authorized access. The content of this role-based training will be updated at least annually and after any organization-defined events that necessitate changes in the training content."</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="49" t="inlineStr">
@@ -18874,12 +19266,36 @@
           <t>Determine if lessons learned from internal or external security incidents or breaches are incorporated into role-based training</t>
         </is>
       </c>
-      <c r="F20" s="77" t="n"/>
-      <c r="G20" s="77" t="n"/>
-      <c r="H20" s="77" t="n"/>
-      <c r="I20" s="46" t="n"/>
-      <c r="J20" s="77" t="n"/>
-      <c r="K20" s="77" t="n"/>
+      <c r="F20" s="89" t="inlineStr">
+        <is>
+          <t>Security-Awareness-and-Training-Policy-Revised.pdf</t>
+        </is>
+      </c>
+      <c r="G20" s="89" t="inlineStr">
+        <is>
+          <t>The provided documents do not contain any sections that specifically mention incorporating lessons learned from internal or external security incidents or breaches into role-based training.</t>
+        </is>
+      </c>
+      <c r="H20" s="89" t="inlineStr">
+        <is>
+          <t>The documents do not meet the requirements of the given test procedure as they do not mention the incorporation of lessons learned from security incidents into role-based training.</t>
+        </is>
+      </c>
+      <c r="I20" s="46" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J20" s="89" t="inlineStr">
+        <is>
+          <t>The organization should incorporate a process for learning from security incidents into their training policy. This could include a review of incidents and breaches, analysis of what went wrong, and how to prevent similar incidents in the future. This information should then be incorporated into role-based training to ensure all staff are aware and can act accordingly.</t>
+        </is>
+      </c>
+      <c r="K20" s="89" t="inlineStr">
+        <is>
+          <t>"Purdue Pharma shall: a. Review and analyze internal and external security incidents and breaches. b. Incorporate lessons learned from these incidents into role-based training. c. Update training materials regularly to reflect recent incidents and prevention strategies."</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="49" t="inlineStr">
@@ -18915,12 +19331,12 @@
       </c>
       <c r="G21" s="89" t="inlineStr">
         <is>
-          <t>"SECURITY TRAINING RECORDS Purdue Pharma shall: a.Designate personnel to document and monitor individual information system security training activities including basic security awareness training and specific information system security training. b.Retain individual training records for six years."</t>
+          <t>"SECURITY AWARENESS TRAINING Purdue Pharma shall: a.Schedule security awareness training as part of initial training for new users. b.Schedule security awareness training when required by information system changes and then every two years thereafter. c.IT shall determine the appropriate content of security awareness training and security awareness techniques based on the specific organizational requirements and the information systems to which personnel have authorized access."; "SECURITY TRAINING RECORDS Purdue Pharma shall: a.Designate personnel to document and monitor individual information system security training activities including basic security awareness training and specific information system security training. b.Retain individual training records for six years."</t>
         </is>
       </c>
       <c r="H21" s="89" t="inlineStr">
         <is>
-          <t>The document clearly states that Purdue Pharma has a policy to document and monitor individual information system security training activities, which includes basic security awareness training and specific information system security training. However, the document does not provide any information about privacy training activities.</t>
+          <t>The document outlines that Purdue Pharma schedules security awareness training for new users and every two years thereafter. It also mentions that the IT department determines the content of the training based on organizational requirements and authorized access. The document also states that Purdue Pharma designates personnel to document and monitor individual information system security training activities and retains these records for six years. However, the document does not mention any specific role-based security training or any privacy awareness training or role-based privacy training.</t>
         </is>
       </c>
       <c r="I21" s="46" t="inlineStr">
@@ -18930,12 +19346,12 @@
       </c>
       <c r="J21" s="89" t="inlineStr">
         <is>
-          <t>The policy should be updated to include provisions for documenting and monitoring privacy training activities. This could include basic privacy awareness training and specific role-based privacy training.</t>
+          <t>Purdue Pharma should implement specific role-based security training and document and monitor these activities. Additionally, Purdue Pharma should also implement privacy awareness training and specific role-based privacy training and document and monitor these activities.</t>
         </is>
       </c>
       <c r="K21" s="89" t="inlineStr">
         <is>
-          <t>"SECURITY AND PRIVACY TRAINING RECORDS Purdue Pharma shall: a.Designate personnel to document and monitor individual information system security and privacy training activities including basic security and privacy awareness training and specific information system security and role-based privacy training. b.Retain individual training records for six years."</t>
+          <t>"SECURITY AWARENESS TRAINING Purdue Pharma shall: a.Schedule security awareness training and specific role-based security training as part of initial training for new users. b.Schedule security awareness training and specific role-based security training when required by information system changes and then every two years thereafter. c.IT shall determine the appropriate content of security awareness training, specific role-based security training, privacy awareness training, and specific role-based privacy training based on the specific organizational requirements and the information systems to which personnel have authorized access."; "SECURITY TRAINING RECORDS Purdue Pharma shall: a.Designate personnel to document and monitor individual information system security training activities including basic security awareness training, specific role-based security training, privacy awareness training, and specific role-based privacy training. b.Retain individual training records for six years."</t>
         </is>
       </c>
     </row>
@@ -18972,12 +19388,12 @@
       </c>
       <c r="G22" s="89" t="inlineStr">
         <is>
-          <t>"SECURITY TRAINING RECORDS Purdue Pharma shall: a.Designate personnel to document and monitor individual information system security training activities including basic security awareness training and specific information system security training. b.Retain individual training records for six years."</t>
+          <t>"SECURITY TRAINING RECORDS Purdue Pharma shall: b.Retain individual training records for six years."</t>
         </is>
       </c>
       <c r="H22" s="89" t="inlineStr">
         <is>
-          <t>The document meets the requirements of the given test procedure. It states that Purdue Pharma will retain individual training records for six years, which is significantly longer than the one year required by the test procedure.</t>
+          <t>The document exceeds the requirements of the given test procedure. The test procedure requires individual security and awareness training records to be retained for at least one year or one year after completion of a specific training program. The document states that Purdue Pharma retains these records for six years.</t>
         </is>
       </c>
       <c r="I22" s="46" t="inlineStr">

</xml_diff>